<commit_message>
Update BP by Adam
</commit_message>
<xml_diff>
--- a/Dokumentasi/Activity Plan/AP WeBooList.xlsx
+++ b/Dokumentasi/Activity Plan/AP WeBooList.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MyWeBooList\Dokumentasi\Activity Plan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC357BAA-D162-4B32-B273-399B829B59AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7845"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACTIVITY PLAN" sheetId="1" r:id="rId1"/>
@@ -196,7 +202,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -896,129 +902,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1060,47 +943,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1112,6 +959,165 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1390,17 +1396,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="B1:EB69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="7" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="7" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
+      <selection pane="bottomRight" activeCell="AS46" sqref="AS46:AX52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,40 +1467,40 @@
       <c r="AG1" s="1"/>
     </row>
     <row r="2" spans="2:132" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="98"/>
+      <c r="AG2" s="98"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
@@ -1596,38 +1602,38 @@
       <c r="EB2" s="1"/>
     </row>
     <row r="3" spans="2:132" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="36"/>
-      <c r="AC3" s="36"/>
-      <c r="AD3" s="36"/>
-      <c r="AE3" s="36"/>
-      <c r="AF3" s="36"/>
-      <c r="AG3" s="36"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
+      <c r="T3" s="98"/>
+      <c r="U3" s="98"/>
+      <c r="V3" s="98"/>
+      <c r="W3" s="98"/>
+      <c r="X3" s="98"/>
+      <c r="Y3" s="98"/>
+      <c r="Z3" s="98"/>
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="98"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="98"/>
+      <c r="AF3" s="98"/>
+      <c r="AG3" s="98"/>
     </row>
     <row r="4" spans="2:132" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -1664,137 +1670,137 @@
       <c r="AG4" s="2"/>
     </row>
     <row r="5" spans="2:132" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="47" t="s">
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="48"/>
-      <c r="Z5" s="49"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="82"/>
+      <c r="Z5" s="83"/>
     </row>
     <row r="6" spans="2:132" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="68" t="s">
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="40" t="s">
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="41"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="40" t="s">
+      <c r="M6" s="72"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="40" t="s">
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="U6" s="41"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="50" t="s">
+      <c r="U6" s="72"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="X6" s="50" t="s">
+      <c r="X6" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="Y6" s="50" t="s">
+      <c r="Y6" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="Z6" s="50" t="s">
+      <c r="Z6" s="84" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:132" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="74">
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="33">
         <v>4</v>
       </c>
-      <c r="H7" s="79">
+      <c r="H7" s="38">
         <v>1</v>
       </c>
-      <c r="I7" s="80">
+      <c r="I7" s="39">
         <v>2</v>
       </c>
-      <c r="J7" s="80">
+      <c r="J7" s="39">
         <v>3</v>
       </c>
-      <c r="K7" s="81">
+      <c r="K7" s="40">
         <v>4</v>
       </c>
-      <c r="L7" s="79">
+      <c r="L7" s="38">
         <v>1</v>
       </c>
-      <c r="M7" s="80">
+      <c r="M7" s="39">
         <v>2</v>
       </c>
-      <c r="N7" s="90">
+      <c r="N7" s="48">
         <v>3</v>
       </c>
-      <c r="O7" s="84">
+      <c r="O7" s="43">
         <v>4</v>
       </c>
-      <c r="P7" s="79">
+      <c r="P7" s="38">
         <v>1</v>
       </c>
-      <c r="Q7" s="80">
+      <c r="Q7" s="39">
         <v>2</v>
       </c>
-      <c r="R7" s="80">
+      <c r="R7" s="39">
         <v>3</v>
       </c>
-      <c r="S7" s="81">
+      <c r="S7" s="40">
         <v>4</v>
       </c>
-      <c r="T7" s="69">
+      <c r="T7" s="28">
         <v>1</v>
       </c>
       <c r="U7" s="17">
@@ -1803,28 +1809,28 @@
       <c r="V7" s="17">
         <v>3</v>
       </c>
-      <c r="W7" s="51"/>
-      <c r="X7" s="51"/>
-      <c r="Y7" s="51"/>
-      <c r="Z7" s="51"/>
+      <c r="W7" s="85"/>
+      <c r="X7" s="85"/>
+      <c r="Y7" s="85"/>
+      <c r="Z7" s="85"/>
     </row>
     <row r="8" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="31">
+      <c r="B8" s="105">
         <v>1</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="56" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="75"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
       <c r="J8" s="14"/>
@@ -1832,28 +1838,28 @@
       <c r="L8" s="15"/>
       <c r="M8" s="14"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="85"/>
+      <c r="O8" s="44"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="70"/>
+      <c r="T8" s="29"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
-      <c r="W8" s="56"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="58"/>
-      <c r="Z8" s="63"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="64"/>
     </row>
     <row r="9" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="45"/>
+      <c r="B9" s="106"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="83"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
       <c r="J9" s="14"/>
@@ -1861,36 +1867,36 @@
       <c r="L9" s="15"/>
       <c r="M9" s="14"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="85"/>
+      <c r="O9" s="44"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="70"/>
+      <c r="T9" s="29"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
-      <c r="W9" s="57"/>
-      <c r="X9" s="59"/>
-      <c r="Y9" s="59"/>
-      <c r="Z9" s="64"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="70"/>
+      <c r="Y9" s="70"/>
+      <c r="Z9" s="75"/>
     </row>
     <row r="10" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="33">
+      <c r="B10" s="107">
         <v>2</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="56" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="76"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="12"/>
       <c r="I10" s="5"/>
       <c r="J10" s="14"/>
@@ -1898,28 +1904,28 @@
       <c r="L10" s="15"/>
       <c r="M10" s="14"/>
       <c r="N10" s="6"/>
-      <c r="O10" s="86"/>
+      <c r="O10" s="45"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="5"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="70"/>
+      <c r="T10" s="29"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="59"/>
-      <c r="Y10" s="59"/>
-      <c r="Z10" s="64"/>
+      <c r="W10" s="80"/>
+      <c r="X10" s="70"/>
+      <c r="Y10" s="70"/>
+      <c r="Z10" s="75"/>
     </row>
     <row r="11" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="45"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="57"/>
       <c r="F11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="76"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="4"/>
       <c r="I11" s="5"/>
       <c r="J11" s="14"/>
@@ -1927,24 +1933,24 @@
       <c r="L11" s="15"/>
       <c r="M11" s="14"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="85"/>
+      <c r="O11" s="44"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="3"/>
-      <c r="T11" s="70"/>
+      <c r="T11" s="29"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="59"/>
-      <c r="Y11" s="59"/>
-      <c r="Z11" s="64"/>
+      <c r="W11" s="80"/>
+      <c r="X11" s="70"/>
+      <c r="Y11" s="70"/>
+      <c r="Z11" s="75"/>
     </row>
     <row r="12" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="26">
+      <c r="B12" s="102">
         <v>3</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="65" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="94" t="s">
@@ -1956,36 +1962,36 @@
       <c r="F12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="76"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="103"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="14"/>
       <c r="K12" s="16"/>
       <c r="L12" s="15"/>
       <c r="M12" s="14"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="85"/>
+      <c r="O12" s="44"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="70"/>
+      <c r="T12" s="29"/>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
-      <c r="W12" s="98"/>
-      <c r="X12" s="99"/>
-      <c r="Y12" s="99"/>
-      <c r="Z12" s="100"/>
+      <c r="W12" s="59"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="61"/>
+      <c r="Z12" s="63"/>
     </row>
     <row r="13" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
-      <c r="C13" s="97"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="95"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="91" t="s">
+      <c r="E13" s="57"/>
+      <c r="F13" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="76"/>
+      <c r="G13" s="35"/>
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
       <c r="J13" s="14"/>
@@ -1993,34 +1999,34 @@
       <c r="L13" s="15"/>
       <c r="M13" s="14"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="85"/>
+      <c r="O13" s="44"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="70"/>
+      <c r="T13" s="29"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="63"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="64"/>
     </row>
     <row r="14" spans="2:132" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="33">
+      <c r="B14" s="107">
         <v>4</v>
       </c>
-      <c r="C14" s="97"/>
-      <c r="D14" s="34" t="s">
+      <c r="C14" s="66"/>
+      <c r="D14" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="56" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="76"/>
+      <c r="G14" s="35"/>
       <c r="H14" s="4"/>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
@@ -2028,28 +2034,28 @@
       <c r="L14" s="15"/>
       <c r="M14" s="14"/>
       <c r="N14" s="5"/>
-      <c r="O14" s="85"/>
+      <c r="O14" s="44"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="70"/>
+      <c r="T14" s="29"/>
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="59"/>
-      <c r="Y14" s="59"/>
-      <c r="Z14" s="64"/>
+      <c r="W14" s="80"/>
+      <c r="X14" s="70"/>
+      <c r="Y14" s="70"/>
+      <c r="Z14" s="75"/>
     </row>
     <row r="15" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="33"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="45"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="76"/>
+      <c r="G15" s="35"/>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
       <c r="J15" s="14"/>
@@ -2057,36 +2063,36 @@
       <c r="L15" s="15"/>
       <c r="M15" s="14"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="85"/>
+      <c r="O15" s="44"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="70"/>
+      <c r="T15" s="29"/>
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
-      <c r="W15" s="57"/>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="64"/>
+      <c r="W15" s="80"/>
+      <c r="X15" s="70"/>
+      <c r="Y15" s="70"/>
+      <c r="Z15" s="75"/>
     </row>
     <row r="16" spans="2:132" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="25">
+      <c r="B16" s="58">
         <v>5</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="104" t="s">
+      <c r="F16" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="76"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="4"/>
       <c r="I16" s="5"/>
       <c r="J16" s="13"/>
@@ -2094,28 +2100,28 @@
       <c r="L16" s="15"/>
       <c r="M16" s="14"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="85"/>
+      <c r="O16" s="44"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="70"/>
+      <c r="T16" s="29"/>
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
-      <c r="W16" s="98"/>
-      <c r="X16" s="99"/>
-      <c r="Y16" s="99"/>
-      <c r="Z16" s="100"/>
+      <c r="W16" s="59"/>
+      <c r="X16" s="61"/>
+      <c r="Y16" s="61"/>
+      <c r="Z16" s="63"/>
     </row>
     <row r="17" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="25"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="105" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="76"/>
+      <c r="G17" s="35"/>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
       <c r="J17" s="14"/>
@@ -2123,34 +2129,34 @@
       <c r="L17" s="15"/>
       <c r="M17" s="14"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="85"/>
+      <c r="O17" s="44"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="70"/>
+      <c r="T17" s="29"/>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="58"/>
-      <c r="Y17" s="58"/>
-      <c r="Z17" s="63"/>
+      <c r="W17" s="60"/>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="62"/>
+      <c r="Z17" s="64"/>
     </row>
     <row r="18" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="25">
+      <c r="B18" s="58">
         <v>6</v>
       </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="66"/>
+      <c r="D18" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="104" t="s">
+      <c r="F18" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="76"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="4"/>
       <c r="I18" s="5"/>
       <c r="J18" s="13"/>
@@ -2158,28 +2164,28 @@
       <c r="L18" s="15"/>
       <c r="M18" s="14"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="85"/>
+      <c r="O18" s="44"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="3"/>
-      <c r="T18" s="70"/>
+      <c r="T18" s="29"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
-      <c r="W18" s="98"/>
-      <c r="X18" s="99"/>
-      <c r="Y18" s="99"/>
-      <c r="Z18" s="100"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="63"/>
     </row>
     <row r="19" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="105" t="s">
+      <c r="B19" s="58"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="76"/>
+      <c r="G19" s="35"/>
       <c r="H19" s="4"/>
       <c r="I19" s="5"/>
       <c r="J19" s="14"/>
@@ -2187,34 +2193,34 @@
       <c r="L19" s="15"/>
       <c r="M19" s="14"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="85"/>
+      <c r="O19" s="44"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="3"/>
-      <c r="T19" s="70"/>
+      <c r="T19" s="29"/>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="58"/>
-      <c r="Y19" s="58"/>
-      <c r="Z19" s="63"/>
+      <c r="W19" s="60"/>
+      <c r="X19" s="62"/>
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="64"/>
     </row>
     <row r="20" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="25">
+      <c r="B20" s="58">
         <v>7</v>
       </c>
-      <c r="C20" s="97"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="66"/>
+      <c r="D20" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="104" t="s">
+      <c r="F20" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="76"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="4"/>
       <c r="I20" s="5"/>
       <c r="J20" s="13"/>
@@ -2222,28 +2228,28 @@
       <c r="L20" s="15"/>
       <c r="M20" s="14"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="85"/>
+      <c r="O20" s="44"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="70"/>
+      <c r="T20" s="29"/>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
-      <c r="W20" s="98"/>
-      <c r="X20" s="99"/>
-      <c r="Y20" s="99"/>
-      <c r="Z20" s="100"/>
+      <c r="W20" s="59"/>
+      <c r="X20" s="61"/>
+      <c r="Y20" s="61"/>
+      <c r="Z20" s="63"/>
     </row>
     <row r="21" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
-      <c r="C21" s="97"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="105" t="s">
+      <c r="B21" s="58"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="76"/>
+      <c r="G21" s="35"/>
       <c r="H21" s="4"/>
       <c r="I21" s="5"/>
       <c r="J21" s="14"/>
@@ -2251,63 +2257,63 @@
       <c r="L21" s="15"/>
       <c r="M21" s="14"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="85"/>
+      <c r="O21" s="44"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="3"/>
-      <c r="T21" s="70"/>
+      <c r="T21" s="29"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="58"/>
-      <c r="Y21" s="58"/>
-      <c r="Z21" s="63"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="62"/>
+      <c r="Y21" s="62"/>
+      <c r="Z21" s="64"/>
     </row>
     <row r="22" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="25">
+      <c r="B22" s="58">
         <v>8</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="66"/>
+      <c r="D22" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="104" t="s">
+      <c r="F22" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="76"/>
+      <c r="G22" s="35"/>
       <c r="H22" s="4"/>
       <c r="I22" s="5"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="82"/>
+      <c r="K22" s="41"/>
       <c r="L22" s="15"/>
       <c r="M22" s="14"/>
       <c r="N22" s="5"/>
-      <c r="O22" s="85"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="3"/>
-      <c r="T22" s="70"/>
+      <c r="T22" s="29"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
-      <c r="W22" s="98"/>
-      <c r="X22" s="99"/>
-      <c r="Y22" s="99"/>
-      <c r="Z22" s="100"/>
+      <c r="W22" s="59"/>
+      <c r="X22" s="61"/>
+      <c r="Y22" s="61"/>
+      <c r="Z22" s="63"/>
     </row>
     <row r="23" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-      <c r="C23" s="97"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="105" t="s">
+      <c r="B23" s="58"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="76"/>
+      <c r="G23" s="35"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
       <c r="J23" s="14"/>
@@ -2315,63 +2321,63 @@
       <c r="L23" s="15"/>
       <c r="M23" s="14"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="85"/>
+      <c r="O23" s="44"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="3"/>
-      <c r="T23" s="70"/>
+      <c r="T23" s="29"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="58"/>
-      <c r="Y23" s="58"/>
-      <c r="Z23" s="63"/>
+      <c r="W23" s="60"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="62"/>
+      <c r="Z23" s="64"/>
     </row>
     <row r="24" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="25">
+      <c r="B24" s="58">
         <v>9</v>
       </c>
-      <c r="C24" s="97"/>
-      <c r="D24" s="25" t="s">
+      <c r="C24" s="66"/>
+      <c r="D24" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="104" t="s">
+      <c r="F24" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="76"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="4"/>
       <c r="I24" s="5"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="82"/>
+      <c r="K24" s="41"/>
       <c r="L24" s="15"/>
       <c r="M24" s="14"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="85"/>
+      <c r="O24" s="44"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="3"/>
-      <c r="T24" s="70"/>
+      <c r="T24" s="29"/>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
-      <c r="W24" s="98"/>
-      <c r="X24" s="99"/>
-      <c r="Y24" s="99"/>
-      <c r="Z24" s="100"/>
+      <c r="W24" s="59"/>
+      <c r="X24" s="61"/>
+      <c r="Y24" s="61"/>
+      <c r="Z24" s="63"/>
     </row>
     <row r="25" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="105" t="s">
+      <c r="B25" s="58"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G25" s="76"/>
+      <c r="G25" s="35"/>
       <c r="H25" s="4"/>
       <c r="I25" s="5"/>
       <c r="J25" s="14"/>
@@ -2379,63 +2385,63 @@
       <c r="L25" s="15"/>
       <c r="M25" s="14"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="85"/>
+      <c r="O25" s="44"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="3"/>
-      <c r="T25" s="70"/>
+      <c r="T25" s="29"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="63"/>
+      <c r="W25" s="60"/>
+      <c r="X25" s="62"/>
+      <c r="Y25" s="62"/>
+      <c r="Z25" s="64"/>
     </row>
     <row r="26" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="31">
+      <c r="B26" s="105">
         <v>4</v>
       </c>
-      <c r="C26" s="97"/>
-      <c r="D26" s="93" t="s">
+      <c r="C26" s="66"/>
+      <c r="D26" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="101" t="s">
+      <c r="E26" s="87" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G26" s="76"/>
+      <c r="G26" s="35"/>
       <c r="H26" s="4"/>
       <c r="I26" s="5"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="82"/>
+      <c r="K26" s="41"/>
       <c r="L26" s="15"/>
       <c r="M26" s="14"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="85"/>
+      <c r="O26" s="44"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="3"/>
-      <c r="T26" s="70"/>
+      <c r="T26" s="29"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
-      <c r="W26" s="57"/>
-      <c r="X26" s="59"/>
-      <c r="Y26" s="59"/>
-      <c r="Z26" s="64"/>
+      <c r="W26" s="80"/>
+      <c r="X26" s="70"/>
+      <c r="Y26" s="70"/>
+      <c r="Z26" s="75"/>
     </row>
     <row r="27" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="32"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="54"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="88"/>
       <c r="F27" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="76"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="4"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -2443,63 +2449,63 @@
       <c r="L27" s="15"/>
       <c r="M27" s="14"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="85"/>
+      <c r="O27" s="44"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="3"/>
-      <c r="T27" s="70"/>
+      <c r="T27" s="29"/>
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
-      <c r="W27" s="57"/>
-      <c r="X27" s="59"/>
-      <c r="Y27" s="59"/>
-      <c r="Z27" s="64"/>
+      <c r="W27" s="80"/>
+      <c r="X27" s="70"/>
+      <c r="Y27" s="70"/>
+      <c r="Z27" s="75"/>
     </row>
     <row r="28" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="25">
+      <c r="B28" s="58">
         <v>5</v>
       </c>
-      <c r="C28" s="97"/>
-      <c r="D28" s="28" t="s">
+      <c r="C28" s="66"/>
+      <c r="D28" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="53" t="s">
+      <c r="E28" s="89" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="76"/>
+      <c r="G28" s="35"/>
       <c r="H28" s="4"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="106"/>
+      <c r="L28" s="53"/>
       <c r="M28" s="14"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="85"/>
+      <c r="O28" s="44"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="3"/>
-      <c r="T28" s="70"/>
+      <c r="T28" s="29"/>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
-      <c r="W28" s="57"/>
-      <c r="X28" s="59"/>
-      <c r="Y28" s="59"/>
-      <c r="Z28" s="64"/>
+      <c r="W28" s="80"/>
+      <c r="X28" s="70"/>
+      <c r="Y28" s="70"/>
+      <c r="Z28" s="75"/>
     </row>
     <row r="29" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="54"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="88"/>
       <c r="F29" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="76"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="4"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -2507,34 +2513,34 @@
       <c r="L29" s="15"/>
       <c r="M29" s="14"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="85"/>
+      <c r="O29" s="44"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="3"/>
-      <c r="T29" s="70"/>
+      <c r="T29" s="29"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="57"/>
-      <c r="X29" s="59"/>
-      <c r="Y29" s="59"/>
-      <c r="Z29" s="64"/>
+      <c r="W29" s="80"/>
+      <c r="X29" s="70"/>
+      <c r="Y29" s="70"/>
+      <c r="Z29" s="75"/>
     </row>
     <row r="30" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="25">
+      <c r="B30" s="58">
         <v>6</v>
       </c>
-      <c r="C30" s="97"/>
-      <c r="D30" s="28" t="s">
+      <c r="C30" s="66"/>
+      <c r="D30" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="53" t="s">
+      <c r="E30" s="89" t="s">
         <v>52</v>
       </c>
       <c r="F30" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="76"/>
+      <c r="G30" s="35"/>
       <c r="H30" s="4"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -2542,28 +2548,28 @@
       <c r="L30" s="12"/>
       <c r="M30" s="14"/>
       <c r="N30" s="5"/>
-      <c r="O30" s="85"/>
+      <c r="O30" s="44"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="3"/>
-      <c r="T30" s="70"/>
+      <c r="T30" s="29"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
-      <c r="W30" s="55"/>
-      <c r="X30" s="52"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="61"/>
+      <c r="W30" s="78"/>
+      <c r="X30" s="68"/>
+      <c r="Y30" s="68"/>
+      <c r="Z30" s="76"/>
     </row>
     <row r="31" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="25"/>
-      <c r="C31" s="97"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="54"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="88"/>
       <c r="F31" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="76"/>
+      <c r="G31" s="35"/>
       <c r="H31" s="4"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -2571,34 +2577,34 @@
       <c r="L31" s="15"/>
       <c r="M31" s="14"/>
       <c r="N31" s="5"/>
-      <c r="O31" s="85"/>
+      <c r="O31" s="44"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="70"/>
+      <c r="T31" s="29"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
-      <c r="W31" s="55"/>
-      <c r="X31" s="52"/>
-      <c r="Y31" s="52"/>
-      <c r="Z31" s="61"/>
+      <c r="W31" s="78"/>
+      <c r="X31" s="68"/>
+      <c r="Y31" s="68"/>
+      <c r="Z31" s="76"/>
     </row>
     <row r="32" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="25">
+      <c r="B32" s="58">
         <v>7</v>
       </c>
-      <c r="C32" s="97"/>
-      <c r="D32" s="28" t="s">
+      <c r="C32" s="66"/>
+      <c r="D32" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="89" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="76"/>
+      <c r="G32" s="35"/>
       <c r="H32" s="4"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
@@ -2606,28 +2612,28 @@
       <c r="L32" s="12"/>
       <c r="M32" s="14"/>
       <c r="N32" s="5"/>
-      <c r="O32" s="85"/>
+      <c r="O32" s="44"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="3"/>
-      <c r="T32" s="70"/>
+      <c r="T32" s="29"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
-      <c r="W32" s="55"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="61"/>
+      <c r="W32" s="78"/>
+      <c r="X32" s="68"/>
+      <c r="Y32" s="68"/>
+      <c r="Z32" s="76"/>
     </row>
     <row r="33" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="25"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="54"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="88"/>
       <c r="F33" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G33" s="77"/>
+      <c r="G33" s="36"/>
       <c r="H33" s="15"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
@@ -2635,34 +2641,34 @@
       <c r="L33" s="15"/>
       <c r="M33" s="14"/>
       <c r="N33" s="14"/>
-      <c r="O33" s="87"/>
+      <c r="O33" s="46"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="14"/>
       <c r="R33" s="14"/>
       <c r="S33" s="16"/>
-      <c r="T33" s="72"/>
+      <c r="T33" s="31"/>
       <c r="U33" s="14"/>
       <c r="V33" s="14"/>
-      <c r="W33" s="55"/>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52"/>
-      <c r="Z33" s="61"/>
+      <c r="W33" s="78"/>
+      <c r="X33" s="68"/>
+      <c r="Y33" s="68"/>
+      <c r="Z33" s="76"/>
     </row>
     <row r="34" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="25">
+      <c r="B34" s="58">
         <v>8</v>
       </c>
-      <c r="C34" s="97"/>
-      <c r="D34" s="28" t="s">
+      <c r="C34" s="66"/>
+      <c r="D34" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="53" t="s">
+      <c r="E34" s="89" t="s">
         <v>51</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="77"/>
+      <c r="G34" s="36"/>
       <c r="H34" s="15"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
@@ -2670,28 +2676,28 @@
       <c r="L34" s="15"/>
       <c r="M34" s="13"/>
       <c r="N34" s="14"/>
-      <c r="O34" s="87"/>
+      <c r="O34" s="46"/>
       <c r="P34" s="15"/>
       <c r="Q34" s="14"/>
       <c r="R34" s="14"/>
       <c r="S34" s="16"/>
-      <c r="T34" s="72"/>
+      <c r="T34" s="31"/>
       <c r="U34" s="14"/>
       <c r="V34" s="14"/>
-      <c r="W34" s="55"/>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52"/>
-      <c r="Z34" s="61"/>
+      <c r="W34" s="78"/>
+      <c r="X34" s="68"/>
+      <c r="Y34" s="68"/>
+      <c r="Z34" s="76"/>
     </row>
     <row r="35" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="25"/>
-      <c r="C35" s="97"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="54"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="88"/>
       <c r="F35" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="77"/>
+      <c r="G35" s="36"/>
       <c r="H35" s="15"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
@@ -2699,36 +2705,36 @@
       <c r="L35" s="15"/>
       <c r="M35" s="14"/>
       <c r="N35" s="14"/>
-      <c r="O35" s="87"/>
+      <c r="O35" s="46"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="14"/>
       <c r="R35" s="14"/>
       <c r="S35" s="16"/>
-      <c r="T35" s="72"/>
+      <c r="T35" s="31"/>
       <c r="U35" s="14"/>
       <c r="V35" s="14"/>
-      <c r="W35" s="55"/>
-      <c r="X35" s="52"/>
-      <c r="Y35" s="52"/>
-      <c r="Z35" s="61"/>
+      <c r="W35" s="78"/>
+      <c r="X35" s="68"/>
+      <c r="Y35" s="68"/>
+      <c r="Z35" s="76"/>
     </row>
     <row r="36" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="26">
+      <c r="B36" s="102">
         <v>9</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="53" t="s">
+      <c r="E36" s="89" t="s">
         <v>52</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G36" s="77"/>
+      <c r="G36" s="36"/>
       <c r="H36" s="15"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
@@ -2736,28 +2742,28 @@
       <c r="L36" s="15"/>
       <c r="M36" s="14"/>
       <c r="N36" s="13"/>
-      <c r="O36" s="87"/>
+      <c r="O36" s="46"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="14"/>
       <c r="R36" s="14"/>
       <c r="S36" s="16"/>
-      <c r="T36" s="72"/>
+      <c r="T36" s="31"/>
       <c r="U36" s="14"/>
       <c r="V36" s="14"/>
-      <c r="W36" s="55"/>
-      <c r="X36" s="52"/>
-      <c r="Y36" s="52"/>
-      <c r="Z36" s="61"/>
+      <c r="W36" s="78"/>
+      <c r="X36" s="68"/>
+      <c r="Y36" s="68"/>
+      <c r="Z36" s="76"/>
     </row>
     <row r="37" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="53"/>
+      <c r="B37" s="103"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="89"/>
       <c r="F37" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G37" s="77"/>
+      <c r="G37" s="36"/>
       <c r="H37" s="15"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
@@ -2765,34 +2771,34 @@
       <c r="L37" s="15"/>
       <c r="M37" s="14"/>
       <c r="N37" s="14"/>
-      <c r="O37" s="87"/>
+      <c r="O37" s="46"/>
       <c r="P37" s="15"/>
       <c r="Q37" s="14"/>
       <c r="R37" s="14"/>
       <c r="S37" s="16"/>
-      <c r="T37" s="72"/>
+      <c r="T37" s="31"/>
       <c r="U37" s="14"/>
       <c r="V37" s="14"/>
-      <c r="W37" s="55"/>
-      <c r="X37" s="52"/>
-      <c r="Y37" s="52"/>
-      <c r="Z37" s="61"/>
+      <c r="W37" s="78"/>
+      <c r="X37" s="68"/>
+      <c r="Y37" s="68"/>
+      <c r="Z37" s="76"/>
     </row>
     <row r="38" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="25">
+      <c r="B38" s="58">
         <v>10</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28" t="s">
+      <c r="C38" s="67"/>
+      <c r="D38" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="43" t="s">
+      <c r="E38" s="90" t="s">
         <v>51</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="77"/>
+      <c r="G38" s="36"/>
       <c r="H38" s="15"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -2800,28 +2806,28 @@
       <c r="L38" s="15"/>
       <c r="M38" s="14"/>
       <c r="N38" s="14"/>
-      <c r="O38" s="107"/>
+      <c r="O38" s="54"/>
       <c r="P38" s="15"/>
       <c r="Q38" s="14"/>
       <c r="R38" s="14"/>
       <c r="S38" s="16"/>
-      <c r="T38" s="72"/>
+      <c r="T38" s="31"/>
       <c r="U38" s="14"/>
       <c r="V38" s="14"/>
-      <c r="W38" s="55"/>
-      <c r="X38" s="52"/>
-      <c r="Y38" s="52"/>
-      <c r="Z38" s="61"/>
+      <c r="W38" s="78"/>
+      <c r="X38" s="68"/>
+      <c r="Y38" s="68"/>
+      <c r="Z38" s="76"/>
     </row>
     <row r="39" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="25"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="35"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="91"/>
       <c r="F39" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G39" s="77"/>
+      <c r="G39" s="36"/>
       <c r="H39" s="15"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -2829,34 +2835,34 @@
       <c r="L39" s="15"/>
       <c r="M39" s="14"/>
       <c r="N39" s="14"/>
-      <c r="O39" s="87"/>
+      <c r="O39" s="46"/>
       <c r="P39" s="15"/>
       <c r="Q39" s="14"/>
       <c r="R39" s="14"/>
       <c r="S39" s="16"/>
-      <c r="T39" s="72"/>
+      <c r="T39" s="31"/>
       <c r="U39" s="14"/>
       <c r="V39" s="14"/>
-      <c r="W39" s="55"/>
-      <c r="X39" s="52"/>
-      <c r="Y39" s="52"/>
-      <c r="Z39" s="61"/>
+      <c r="W39" s="78"/>
+      <c r="X39" s="68"/>
+      <c r="Y39" s="68"/>
+      <c r="Z39" s="76"/>
     </row>
     <row r="40" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="26">
+      <c r="B40" s="102">
         <v>11</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28" t="s">
+      <c r="C40" s="67"/>
+      <c r="D40" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="43" t="s">
+      <c r="E40" s="90" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="77"/>
+      <c r="G40" s="36"/>
       <c r="H40" s="15"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -2864,28 +2870,28 @@
       <c r="L40" s="15"/>
       <c r="M40" s="14"/>
       <c r="N40" s="14"/>
-      <c r="O40" s="87"/>
+      <c r="O40" s="46"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="14"/>
       <c r="R40" s="14"/>
       <c r="S40" s="16"/>
-      <c r="T40" s="72"/>
+      <c r="T40" s="31"/>
       <c r="U40" s="14"/>
       <c r="V40" s="14"/>
-      <c r="W40" s="55"/>
-      <c r="X40" s="52"/>
-      <c r="Y40" s="52"/>
-      <c r="Z40" s="61"/>
+      <c r="W40" s="78"/>
+      <c r="X40" s="68"/>
+      <c r="Y40" s="68"/>
+      <c r="Z40" s="76"/>
     </row>
     <row r="41" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="27"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="35"/>
+      <c r="B41" s="103"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="91"/>
       <c r="F41" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="77"/>
+      <c r="G41" s="36"/>
       <c r="H41" s="15"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -2893,36 +2899,36 @@
       <c r="L41" s="15"/>
       <c r="M41" s="14"/>
       <c r="N41" s="14"/>
-      <c r="O41" s="87"/>
+      <c r="O41" s="46"/>
       <c r="P41" s="15"/>
       <c r="Q41" s="14"/>
       <c r="R41" s="14"/>
       <c r="S41" s="16"/>
-      <c r="T41" s="72"/>
+      <c r="T41" s="31"/>
       <c r="U41" s="14"/>
       <c r="V41" s="14"/>
-      <c r="W41" s="55"/>
-      <c r="X41" s="52"/>
-      <c r="Y41" s="52"/>
-      <c r="Z41" s="61"/>
+      <c r="W41" s="78"/>
+      <c r="X41" s="68"/>
+      <c r="Y41" s="68"/>
+      <c r="Z41" s="76"/>
     </row>
     <row r="42" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="25">
+      <c r="B42" s="58">
         <v>16</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="102" t="s">
+      <c r="E42" s="86" t="s">
         <v>51</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G42" s="77"/>
+      <c r="G42" s="36"/>
       <c r="H42" s="15"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -2930,28 +2936,28 @@
       <c r="L42" s="15"/>
       <c r="M42" s="14"/>
       <c r="N42" s="14"/>
-      <c r="O42" s="87"/>
+      <c r="O42" s="46"/>
       <c r="P42" s="15"/>
       <c r="Q42" s="13"/>
       <c r="R42" s="14"/>
       <c r="S42" s="16"/>
-      <c r="T42" s="72"/>
+      <c r="T42" s="31"/>
       <c r="U42" s="14"/>
       <c r="V42" s="14"/>
-      <c r="W42" s="55"/>
-      <c r="X42" s="52"/>
-      <c r="Y42" s="52"/>
-      <c r="Z42" s="61"/>
+      <c r="W42" s="78"/>
+      <c r="X42" s="68"/>
+      <c r="Y42" s="68"/>
+      <c r="Z42" s="76"/>
     </row>
     <row r="43" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="25"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="102"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="86"/>
       <c r="F43" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="77"/>
+      <c r="G43" s="36"/>
       <c r="H43" s="15"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -2959,34 +2965,34 @@
       <c r="L43" s="15"/>
       <c r="M43" s="14"/>
       <c r="N43" s="14"/>
-      <c r="O43" s="87"/>
+      <c r="O43" s="46"/>
       <c r="P43" s="15"/>
       <c r="Q43" s="14"/>
       <c r="R43" s="14"/>
       <c r="S43" s="16"/>
-      <c r="T43" s="72"/>
+      <c r="T43" s="31"/>
       <c r="U43" s="14"/>
       <c r="V43" s="14"/>
-      <c r="W43" s="55"/>
-      <c r="X43" s="52"/>
-      <c r="Y43" s="52"/>
-      <c r="Z43" s="61"/>
+      <c r="W43" s="78"/>
+      <c r="X43" s="68"/>
+      <c r="Y43" s="68"/>
+      <c r="Z43" s="76"/>
     </row>
     <row r="44" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="26">
+      <c r="B44" s="102">
         <v>17</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28" t="s">
+      <c r="C44" s="67"/>
+      <c r="D44" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E44" s="67" t="s">
         <v>52</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G44" s="77"/>
+      <c r="G44" s="36"/>
       <c r="H44" s="15"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -2994,28 +3000,28 @@
       <c r="L44" s="15"/>
       <c r="M44" s="14"/>
       <c r="N44" s="14"/>
-      <c r="O44" s="87"/>
+      <c r="O44" s="46"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="14"/>
       <c r="R44" s="13"/>
       <c r="S44" s="16"/>
-      <c r="T44" s="72"/>
+      <c r="T44" s="31"/>
       <c r="U44" s="14"/>
       <c r="V44" s="14"/>
-      <c r="W44" s="55"/>
-      <c r="X44" s="52"/>
-      <c r="Y44" s="52"/>
-      <c r="Z44" s="61"/>
+      <c r="W44" s="78"/>
+      <c r="X44" s="68"/>
+      <c r="Y44" s="68"/>
+      <c r="Z44" s="76"/>
     </row>
     <row r="45" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="B45" s="103"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
       <c r="F45" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G45" s="77"/>
+      <c r="G45" s="36"/>
       <c r="H45" s="15"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -3023,34 +3029,34 @@
       <c r="L45" s="15"/>
       <c r="M45" s="14"/>
       <c r="N45" s="14"/>
-      <c r="O45" s="87"/>
+      <c r="O45" s="46"/>
       <c r="P45" s="15"/>
       <c r="Q45" s="14"/>
       <c r="R45" s="14"/>
       <c r="S45" s="16"/>
-      <c r="T45" s="72"/>
+      <c r="T45" s="31"/>
       <c r="U45" s="14"/>
       <c r="V45" s="14"/>
-      <c r="W45" s="55"/>
-      <c r="X45" s="52"/>
-      <c r="Y45" s="52"/>
-      <c r="Z45" s="61"/>
+      <c r="W45" s="78"/>
+      <c r="X45" s="68"/>
+      <c r="Y45" s="68"/>
+      <c r="Z45" s="76"/>
     </row>
     <row r="46" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="25">
+      <c r="B46" s="58">
         <v>18</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28" t="s">
+      <c r="C46" s="67"/>
+      <c r="D46" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="E46" s="28" t="s">
+      <c r="E46" s="67" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G46" s="77"/>
+      <c r="G46" s="36"/>
       <c r="H46" s="15"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -3058,28 +3064,28 @@
       <c r="L46" s="15"/>
       <c r="M46" s="14"/>
       <c r="N46" s="14"/>
-      <c r="O46" s="87"/>
+      <c r="O46" s="46"/>
       <c r="P46" s="15"/>
       <c r="Q46" s="14"/>
       <c r="R46" s="14"/>
-      <c r="S46" s="82"/>
-      <c r="T46" s="72"/>
+      <c r="S46" s="41"/>
+      <c r="T46" s="31"/>
       <c r="U46" s="14"/>
       <c r="V46" s="14"/>
-      <c r="W46" s="57"/>
-      <c r="X46" s="59"/>
-      <c r="Y46" s="59"/>
-      <c r="Z46" s="64"/>
+      <c r="W46" s="80"/>
+      <c r="X46" s="70"/>
+      <c r="Y46" s="70"/>
+      <c r="Z46" s="75"/>
     </row>
     <row r="47" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="77"/>
+      <c r="G47" s="36"/>
       <c r="H47" s="15"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -3087,36 +3093,36 @@
       <c r="L47" s="15"/>
       <c r="M47" s="14"/>
       <c r="N47" s="14"/>
-      <c r="O47" s="87"/>
+      <c r="O47" s="46"/>
       <c r="P47" s="15"/>
       <c r="Q47" s="14"/>
       <c r="R47" s="14"/>
       <c r="S47" s="16"/>
-      <c r="T47" s="72"/>
+      <c r="T47" s="31"/>
       <c r="U47" s="14"/>
       <c r="V47" s="14"/>
-      <c r="W47" s="57"/>
-      <c r="X47" s="59"/>
-      <c r="Y47" s="59"/>
-      <c r="Z47" s="64"/>
+      <c r="W47" s="80"/>
+      <c r="X47" s="70"/>
+      <c r="Y47" s="70"/>
+      <c r="Z47" s="75"/>
     </row>
     <row r="48" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="26">
+      <c r="B48" s="102">
         <v>19</v>
       </c>
-      <c r="C48" s="97" t="s">
+      <c r="C48" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="28" t="s">
+      <c r="D48" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="28" t="s">
+      <c r="E48" s="67" t="s">
         <v>51</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G48" s="77"/>
+      <c r="G48" s="36"/>
       <c r="H48" s="15"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
@@ -3124,28 +3130,28 @@
       <c r="L48" s="15"/>
       <c r="M48" s="14"/>
       <c r="N48" s="14"/>
-      <c r="O48" s="87"/>
+      <c r="O48" s="46"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="14"/>
       <c r="R48" s="14"/>
       <c r="S48" s="16"/>
-      <c r="T48" s="71"/>
+      <c r="T48" s="30"/>
       <c r="U48" s="14"/>
       <c r="V48" s="14"/>
-      <c r="W48" s="57"/>
-      <c r="X48" s="59"/>
-      <c r="Y48" s="59"/>
-      <c r="Z48" s="64"/>
+      <c r="W48" s="80"/>
+      <c r="X48" s="70"/>
+      <c r="Y48" s="70"/>
+      <c r="Z48" s="75"/>
     </row>
     <row r="49" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="27"/>
-      <c r="C49" s="97"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
       <c r="F49" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G49" s="77"/>
+      <c r="G49" s="36"/>
       <c r="H49" s="15"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
@@ -3153,34 +3159,34 @@
       <c r="L49" s="15"/>
       <c r="M49" s="14"/>
       <c r="N49" s="14"/>
-      <c r="O49" s="87"/>
+      <c r="O49" s="46"/>
       <c r="P49" s="15"/>
       <c r="Q49" s="14"/>
       <c r="R49" s="14"/>
       <c r="S49" s="16"/>
-      <c r="T49" s="72"/>
+      <c r="T49" s="31"/>
       <c r="U49" s="14"/>
       <c r="V49" s="14"/>
-      <c r="W49" s="57"/>
-      <c r="X49" s="59"/>
-      <c r="Y49" s="59"/>
-      <c r="Z49" s="64"/>
+      <c r="W49" s="80"/>
+      <c r="X49" s="70"/>
+      <c r="Y49" s="70"/>
+      <c r="Z49" s="75"/>
     </row>
     <row r="50" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="25">
+      <c r="B50" s="58">
         <v>20</v>
       </c>
-      <c r="C50" s="97"/>
-      <c r="D50" s="28" t="s">
+      <c r="C50" s="66"/>
+      <c r="D50" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="67" t="s">
         <v>52</v>
       </c>
       <c r="F50" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G50" s="77"/>
+      <c r="G50" s="36"/>
       <c r="H50" s="15"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
@@ -3188,28 +3194,28 @@
       <c r="L50" s="15"/>
       <c r="M50" s="14"/>
       <c r="N50" s="14"/>
-      <c r="O50" s="87"/>
+      <c r="O50" s="46"/>
       <c r="P50" s="15"/>
       <c r="Q50" s="14"/>
       <c r="R50" s="14"/>
       <c r="S50" s="16"/>
-      <c r="T50" s="71"/>
+      <c r="T50" s="30"/>
       <c r="U50" s="14"/>
       <c r="V50" s="14"/>
-      <c r="W50" s="57"/>
-      <c r="X50" s="59"/>
-      <c r="Y50" s="59"/>
-      <c r="Z50" s="64"/>
+      <c r="W50" s="80"/>
+      <c r="X50" s="70"/>
+      <c r="Y50" s="70"/>
+      <c r="Z50" s="75"/>
     </row>
     <row r="51" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="25"/>
-      <c r="C51" s="97"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
       <c r="F51" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G51" s="77"/>
+      <c r="G51" s="36"/>
       <c r="H51" s="15"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
@@ -3217,34 +3223,34 @@
       <c r="L51" s="15"/>
       <c r="M51" s="14"/>
       <c r="N51" s="14"/>
-      <c r="O51" s="87"/>
+      <c r="O51" s="46"/>
       <c r="P51" s="15"/>
       <c r="Q51" s="14"/>
       <c r="R51" s="14"/>
       <c r="S51" s="16"/>
-      <c r="T51" s="72"/>
+      <c r="T51" s="31"/>
       <c r="U51" s="14"/>
       <c r="V51" s="14"/>
-      <c r="W51" s="57"/>
-      <c r="X51" s="59"/>
-      <c r="Y51" s="59"/>
-      <c r="Z51" s="64"/>
+      <c r="W51" s="80"/>
+      <c r="X51" s="70"/>
+      <c r="Y51" s="70"/>
+      <c r="Z51" s="75"/>
     </row>
     <row r="52" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="26">
+      <c r="B52" s="102">
         <v>21</v>
       </c>
-      <c r="C52" s="97"/>
-      <c r="D52" s="28" t="s">
+      <c r="C52" s="66"/>
+      <c r="D52" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="67" t="s">
         <v>9</v>
       </c>
       <c r="F52" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G52" s="77"/>
+      <c r="G52" s="36"/>
       <c r="H52" s="15"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
@@ -3252,28 +3258,28 @@
       <c r="L52" s="15"/>
       <c r="M52" s="14"/>
       <c r="N52" s="14"/>
-      <c r="O52" s="87"/>
+      <c r="O52" s="46"/>
       <c r="P52" s="15"/>
       <c r="Q52" s="14"/>
       <c r="R52" s="14"/>
       <c r="S52" s="16"/>
-      <c r="T52" s="71"/>
+      <c r="T52" s="30"/>
       <c r="U52" s="14"/>
       <c r="V52" s="14"/>
-      <c r="W52" s="57"/>
-      <c r="X52" s="59"/>
-      <c r="Y52" s="59"/>
-      <c r="Z52" s="64"/>
+      <c r="W52" s="80"/>
+      <c r="X52" s="70"/>
+      <c r="Y52" s="70"/>
+      <c r="Z52" s="75"/>
     </row>
     <row r="53" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="27"/>
-      <c r="C53" s="93"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="B53" s="103"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
       <c r="F53" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G53" s="77"/>
+      <c r="G53" s="36"/>
       <c r="H53" s="15"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
@@ -3281,36 +3287,36 @@
       <c r="L53" s="15"/>
       <c r="M53" s="14"/>
       <c r="N53" s="14"/>
-      <c r="O53" s="87"/>
+      <c r="O53" s="46"/>
       <c r="P53" s="15"/>
       <c r="Q53" s="14"/>
       <c r="R53" s="14"/>
       <c r="S53" s="16"/>
-      <c r="T53" s="72"/>
+      <c r="T53" s="31"/>
       <c r="U53" s="14"/>
       <c r="V53" s="14"/>
-      <c r="W53" s="57"/>
-      <c r="X53" s="59"/>
-      <c r="Y53" s="59"/>
-      <c r="Z53" s="64"/>
+      <c r="W53" s="80"/>
+      <c r="X53" s="70"/>
+      <c r="Y53" s="70"/>
+      <c r="Z53" s="75"/>
     </row>
     <row r="54" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="25">
+      <c r="B54" s="58">
         <v>22</v>
       </c>
-      <c r="C54" s="92" t="s">
+      <c r="C54" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D54" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="44" t="s">
+      <c r="E54" s="56" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G54" s="77"/>
+      <c r="G54" s="36"/>
       <c r="H54" s="15"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
@@ -3318,28 +3324,28 @@
       <c r="L54" s="15"/>
       <c r="M54" s="14"/>
       <c r="N54" s="14"/>
-      <c r="O54" s="87"/>
+      <c r="O54" s="46"/>
       <c r="P54" s="15"/>
       <c r="Q54" s="14"/>
       <c r="R54" s="14"/>
       <c r="S54" s="16"/>
-      <c r="T54" s="72"/>
+      <c r="T54" s="31"/>
       <c r="U54" s="13"/>
       <c r="V54" s="14"/>
-      <c r="W54" s="57"/>
-      <c r="X54" s="59"/>
-      <c r="Y54" s="59"/>
-      <c r="Z54" s="64"/>
+      <c r="W54" s="80"/>
+      <c r="X54" s="70"/>
+      <c r="Y54" s="70"/>
+      <c r="Z54" s="75"/>
     </row>
     <row r="55" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="25"/>
-      <c r="C55" s="97"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="45"/>
+      <c r="B55" s="58"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="57"/>
       <c r="F55" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G55" s="77"/>
+      <c r="G55" s="36"/>
       <c r="H55" s="15"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
@@ -3347,34 +3353,34 @@
       <c r="L55" s="15"/>
       <c r="M55" s="14"/>
       <c r="N55" s="14"/>
-      <c r="O55" s="87"/>
+      <c r="O55" s="46"/>
       <c r="P55" s="15"/>
       <c r="Q55" s="14"/>
       <c r="R55" s="14"/>
       <c r="S55" s="16"/>
-      <c r="T55" s="72"/>
+      <c r="T55" s="31"/>
       <c r="U55" s="14"/>
       <c r="V55" s="14"/>
-      <c r="W55" s="57"/>
-      <c r="X55" s="59"/>
-      <c r="Y55" s="59"/>
-      <c r="Z55" s="64"/>
+      <c r="W55" s="80"/>
+      <c r="X55" s="70"/>
+      <c r="Y55" s="70"/>
+      <c r="Z55" s="75"/>
     </row>
     <row r="56" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="26">
+      <c r="B56" s="102">
         <v>23</v>
       </c>
-      <c r="C56" s="97"/>
-      <c r="D56" s="28" t="s">
+      <c r="C56" s="66"/>
+      <c r="D56" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="E56" s="44" t="s">
+      <c r="E56" s="56" t="s">
         <v>52</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G56" s="77"/>
+      <c r="G56" s="36"/>
       <c r="H56" s="15"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
@@ -3382,28 +3388,28 @@
       <c r="L56" s="15"/>
       <c r="M56" s="14"/>
       <c r="N56" s="14"/>
-      <c r="O56" s="87"/>
+      <c r="O56" s="46"/>
       <c r="P56" s="15"/>
       <c r="Q56" s="14"/>
       <c r="R56" s="14"/>
       <c r="S56" s="16"/>
-      <c r="T56" s="72"/>
+      <c r="T56" s="31"/>
       <c r="U56" s="13"/>
       <c r="V56" s="14"/>
-      <c r="W56" s="55"/>
-      <c r="X56" s="52"/>
-      <c r="Y56" s="52"/>
-      <c r="Z56" s="61"/>
+      <c r="W56" s="78"/>
+      <c r="X56" s="68"/>
+      <c r="Y56" s="68"/>
+      <c r="Z56" s="76"/>
     </row>
     <row r="57" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="27"/>
-      <c r="C57" s="97"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="45"/>
+      <c r="B57" s="103"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="57"/>
       <c r="F57" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="77"/>
+      <c r="G57" s="36"/>
       <c r="H57" s="15"/>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
@@ -3411,34 +3417,34 @@
       <c r="L57" s="15"/>
       <c r="M57" s="14"/>
       <c r="N57" s="14"/>
-      <c r="O57" s="87"/>
+      <c r="O57" s="46"/>
       <c r="P57" s="15"/>
       <c r="Q57" s="14"/>
       <c r="R57" s="14"/>
       <c r="S57" s="16"/>
-      <c r="T57" s="72"/>
+      <c r="T57" s="31"/>
       <c r="U57" s="14"/>
       <c r="V57" s="14"/>
-      <c r="W57" s="55"/>
-      <c r="X57" s="52"/>
-      <c r="Y57" s="52"/>
-      <c r="Z57" s="61"/>
+      <c r="W57" s="78"/>
+      <c r="X57" s="68"/>
+      <c r="Y57" s="68"/>
+      <c r="Z57" s="76"/>
     </row>
     <row r="58" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="25">
+      <c r="B58" s="58">
         <v>24</v>
       </c>
-      <c r="C58" s="97"/>
-      <c r="D58" s="28" t="s">
+      <c r="C58" s="66"/>
+      <c r="D58" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="E58" s="44" t="s">
+      <c r="E58" s="56" t="s">
         <v>9</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G58" s="77"/>
+      <c r="G58" s="36"/>
       <c r="H58" s="15"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
@@ -3446,28 +3452,28 @@
       <c r="L58" s="15"/>
       <c r="M58" s="14"/>
       <c r="N58" s="14"/>
-      <c r="O58" s="87"/>
+      <c r="O58" s="46"/>
       <c r="P58" s="15"/>
       <c r="Q58" s="14"/>
       <c r="R58" s="14"/>
       <c r="S58" s="16"/>
-      <c r="T58" s="72"/>
+      <c r="T58" s="31"/>
       <c r="U58" s="13"/>
       <c r="V58" s="14"/>
-      <c r="W58" s="55"/>
-      <c r="X58" s="52"/>
-      <c r="Y58" s="52"/>
-      <c r="Z58" s="61"/>
+      <c r="W58" s="78"/>
+      <c r="X58" s="68"/>
+      <c r="Y58" s="68"/>
+      <c r="Z58" s="76"/>
     </row>
     <row r="59" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="25"/>
-      <c r="C59" s="97"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="45"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="57"/>
       <c r="F59" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G59" s="77"/>
+      <c r="G59" s="36"/>
       <c r="H59" s="15"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
@@ -3475,34 +3481,34 @@
       <c r="L59" s="15"/>
       <c r="M59" s="14"/>
       <c r="N59" s="14"/>
-      <c r="O59" s="87"/>
+      <c r="O59" s="46"/>
       <c r="P59" s="15"/>
       <c r="Q59" s="14"/>
       <c r="R59" s="14"/>
       <c r="S59" s="16"/>
-      <c r="T59" s="72"/>
+      <c r="T59" s="31"/>
       <c r="U59" s="14"/>
       <c r="V59" s="14"/>
-      <c r="W59" s="55"/>
-      <c r="X59" s="52"/>
-      <c r="Y59" s="52"/>
-      <c r="Z59" s="61"/>
+      <c r="W59" s="78"/>
+      <c r="X59" s="68"/>
+      <c r="Y59" s="68"/>
+      <c r="Z59" s="76"/>
     </row>
     <row r="60" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="26">
+      <c r="B60" s="102">
         <v>25</v>
       </c>
-      <c r="C60" s="97"/>
-      <c r="D60" s="28" t="s">
+      <c r="C60" s="66"/>
+      <c r="D60" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E60" s="44" t="s">
+      <c r="E60" s="56" t="s">
         <v>51</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G60" s="77"/>
+      <c r="G60" s="36"/>
       <c r="H60" s="15"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
@@ -3510,28 +3516,28 @@
       <c r="L60" s="15"/>
       <c r="M60" s="14"/>
       <c r="N60" s="14"/>
-      <c r="O60" s="87"/>
+      <c r="O60" s="46"/>
       <c r="P60" s="15"/>
       <c r="Q60" s="14"/>
       <c r="R60" s="14"/>
       <c r="S60" s="16"/>
-      <c r="T60" s="72"/>
+      <c r="T60" s="31"/>
       <c r="U60" s="13"/>
       <c r="V60" s="14"/>
-      <c r="W60" s="55"/>
-      <c r="X60" s="52"/>
-      <c r="Y60" s="52"/>
-      <c r="Z60" s="61"/>
+      <c r="W60" s="78"/>
+      <c r="X60" s="68"/>
+      <c r="Y60" s="68"/>
+      <c r="Z60" s="76"/>
     </row>
     <row r="61" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="27"/>
-      <c r="C61" s="97"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="45"/>
+      <c r="B61" s="103"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="57"/>
       <c r="F61" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G61" s="77"/>
+      <c r="G61" s="36"/>
       <c r="H61" s="15"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
@@ -3539,36 +3545,36 @@
       <c r="L61" s="15"/>
       <c r="M61" s="14"/>
       <c r="N61" s="14"/>
-      <c r="O61" s="87"/>
+      <c r="O61" s="46"/>
       <c r="P61" s="15"/>
       <c r="Q61" s="14"/>
       <c r="R61" s="14"/>
       <c r="S61" s="16"/>
-      <c r="T61" s="72"/>
+      <c r="T61" s="31"/>
       <c r="U61" s="14"/>
       <c r="V61" s="14"/>
-      <c r="W61" s="55"/>
-      <c r="X61" s="52"/>
-      <c r="Y61" s="52"/>
-      <c r="Z61" s="61"/>
+      <c r="W61" s="78"/>
+      <c r="X61" s="68"/>
+      <c r="Y61" s="68"/>
+      <c r="Z61" s="76"/>
     </row>
     <row r="62" spans="2:56" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="25">
+      <c r="B62" s="58">
         <v>26</v>
       </c>
-      <c r="C62" s="97" t="s">
+      <c r="C62" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="E62" s="44" t="s">
+      <c r="E62" s="56" t="s">
         <v>52</v>
       </c>
       <c r="F62" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G62" s="77"/>
+      <c r="G62" s="36"/>
       <c r="H62" s="15"/>
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
@@ -3576,28 +3582,28 @@
       <c r="L62" s="15"/>
       <c r="M62" s="14"/>
       <c r="N62" s="14"/>
-      <c r="O62" s="87"/>
+      <c r="O62" s="46"/>
       <c r="P62" s="15"/>
       <c r="Q62" s="14"/>
       <c r="R62" s="14"/>
       <c r="S62" s="16"/>
-      <c r="T62" s="72"/>
+      <c r="T62" s="31"/>
       <c r="U62" s="14"/>
       <c r="V62" s="14"/>
-      <c r="W62" s="55"/>
-      <c r="X62" s="52"/>
-      <c r="Y62" s="52"/>
-      <c r="Z62" s="61"/>
+      <c r="W62" s="78"/>
+      <c r="X62" s="68"/>
+      <c r="Y62" s="68"/>
+      <c r="Z62" s="76"/>
     </row>
     <row r="63" spans="2:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="25"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="45"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="58"/>
+      <c r="E63" s="57"/>
       <c r="F63" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G63" s="78"/>
+      <c r="G63" s="37"/>
       <c r="H63" s="22"/>
       <c r="I63" s="23"/>
       <c r="J63" s="23"/>
@@ -3605,18 +3611,18 @@
       <c r="L63" s="22"/>
       <c r="M63" s="23"/>
       <c r="N63" s="23"/>
-      <c r="O63" s="88"/>
+      <c r="O63" s="47"/>
       <c r="P63" s="22"/>
       <c r="Q63" s="23"/>
       <c r="R63" s="23"/>
       <c r="S63" s="24"/>
-      <c r="T63" s="73"/>
+      <c r="T63" s="32"/>
       <c r="U63" s="23"/>
-      <c r="V63" s="108"/>
-      <c r="W63" s="60"/>
-      <c r="X63" s="62"/>
-      <c r="Y63" s="62"/>
-      <c r="Z63" s="65"/>
+      <c r="V63" s="55"/>
+      <c r="W63" s="79"/>
+      <c r="X63" s="69"/>
+      <c r="Y63" s="69"/>
+      <c r="Z63" s="77"/>
     </row>
     <row r="64" spans="2:56" x14ac:dyDescent="0.25">
       <c r="BC64" s="20"/>
@@ -3644,206 +3650,6 @@
     </row>
   </sheetData>
   <mergeCells count="220">
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="W24:W25"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="Y24:Y25"/>
-    <mergeCell ref="Z24:Z25"/>
-    <mergeCell ref="C16:C35"/>
-    <mergeCell ref="C36:C41"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="W20:W21"/>
-    <mergeCell ref="X20:X21"/>
-    <mergeCell ref="Y20:Y21"/>
-    <mergeCell ref="Z20:Z21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="Y22:Y23"/>
-    <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="X60:X61"/>
-    <mergeCell ref="X62:X63"/>
-    <mergeCell ref="X50:X51"/>
-    <mergeCell ref="X52:X53"/>
-    <mergeCell ref="X54:X55"/>
-    <mergeCell ref="X56:X57"/>
-    <mergeCell ref="X58:X59"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="W12:W13"/>
-    <mergeCell ref="X12:X13"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="X16:X17"/>
-    <mergeCell ref="W18:W19"/>
-    <mergeCell ref="X18:X19"/>
-    <mergeCell ref="Z50:Z51"/>
-    <mergeCell ref="Z52:Z53"/>
-    <mergeCell ref="Z54:Z55"/>
-    <mergeCell ref="Z56:Z57"/>
-    <mergeCell ref="Z58:Z59"/>
-    <mergeCell ref="Z42:Z43"/>
-    <mergeCell ref="Z44:Z45"/>
-    <mergeCell ref="Z46:Z47"/>
-    <mergeCell ref="Z48:Z49"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="Z14:Z15"/>
-    <mergeCell ref="Z26:Z27"/>
-    <mergeCell ref="Z28:Z29"/>
-    <mergeCell ref="Z30:Z31"/>
-    <mergeCell ref="Z32:Z33"/>
-    <mergeCell ref="Z34:Z35"/>
-    <mergeCell ref="Z36:Z37"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="Z18:Z19"/>
-    <mergeCell ref="Z38:Z39"/>
-    <mergeCell ref="Z40:Z41"/>
-    <mergeCell ref="Y60:Y61"/>
-    <mergeCell ref="Y62:Y63"/>
-    <mergeCell ref="Y50:Y51"/>
-    <mergeCell ref="Y52:Y53"/>
-    <mergeCell ref="Y54:Y55"/>
-    <mergeCell ref="Y56:Y57"/>
-    <mergeCell ref="Y58:Y59"/>
-    <mergeCell ref="Y42:Y43"/>
-    <mergeCell ref="Y44:Y45"/>
-    <mergeCell ref="Y46:Y47"/>
-    <mergeCell ref="Y48:Y49"/>
-    <mergeCell ref="Y38:Y39"/>
-    <mergeCell ref="Y40:Y41"/>
-    <mergeCell ref="Z60:Z61"/>
-    <mergeCell ref="Z62:Z63"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="Y14:Y15"/>
-    <mergeCell ref="Y26:Y27"/>
-    <mergeCell ref="Y28:Y29"/>
-    <mergeCell ref="Y30:Y31"/>
-    <mergeCell ref="Y32:Y33"/>
-    <mergeCell ref="Y34:Y35"/>
-    <mergeCell ref="Y36:Y37"/>
-    <mergeCell ref="Y12:Y13"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="Y18:Y19"/>
-    <mergeCell ref="X40:X41"/>
-    <mergeCell ref="X42:X43"/>
-    <mergeCell ref="X30:X31"/>
-    <mergeCell ref="X32:X33"/>
-    <mergeCell ref="X34:X35"/>
-    <mergeCell ref="X36:X37"/>
-    <mergeCell ref="X38:X39"/>
-    <mergeCell ref="X8:X9"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="X14:X15"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="X28:X29"/>
-    <mergeCell ref="W60:W61"/>
-    <mergeCell ref="W62:W63"/>
-    <mergeCell ref="W50:W51"/>
-    <mergeCell ref="W52:W53"/>
-    <mergeCell ref="W54:W55"/>
-    <mergeCell ref="W56:W57"/>
-    <mergeCell ref="W58:W59"/>
-    <mergeCell ref="W42:W43"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="W46:W47"/>
-    <mergeCell ref="W48:W49"/>
-    <mergeCell ref="X44:X45"/>
-    <mergeCell ref="X46:X47"/>
-    <mergeCell ref="X48:X49"/>
-    <mergeCell ref="W40:W41"/>
-    <mergeCell ref="W30:W31"/>
-    <mergeCell ref="W32:W33"/>
-    <mergeCell ref="W34:W35"/>
-    <mergeCell ref="W36:W37"/>
-    <mergeCell ref="W38:W39"/>
-    <mergeCell ref="W8:W9"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="W26:W27"/>
-    <mergeCell ref="W28:W29"/>
-    <mergeCell ref="W5:Z5"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B2:AG3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C54:C61"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="F5:F7"/>
@@ -3864,6 +3670,206 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D28:D29"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C54:C61"/>
+    <mergeCell ref="B2:AG3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="W5:Z5"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="X44:X45"/>
+    <mergeCell ref="X46:X47"/>
+    <mergeCell ref="X48:X49"/>
+    <mergeCell ref="W40:W41"/>
+    <mergeCell ref="W30:W31"/>
+    <mergeCell ref="W32:W33"/>
+    <mergeCell ref="W34:W35"/>
+    <mergeCell ref="W36:W37"/>
+    <mergeCell ref="W38:W39"/>
+    <mergeCell ref="W60:W61"/>
+    <mergeCell ref="W62:W63"/>
+    <mergeCell ref="W50:W51"/>
+    <mergeCell ref="W52:W53"/>
+    <mergeCell ref="W54:W55"/>
+    <mergeCell ref="W56:W57"/>
+    <mergeCell ref="W58:W59"/>
+    <mergeCell ref="W42:W43"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="W46:W47"/>
+    <mergeCell ref="W48:W49"/>
+    <mergeCell ref="X42:X43"/>
+    <mergeCell ref="X30:X31"/>
+    <mergeCell ref="X32:X33"/>
+    <mergeCell ref="X34:X35"/>
+    <mergeCell ref="X36:X37"/>
+    <mergeCell ref="X38:X39"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="X14:X15"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="Y44:Y45"/>
+    <mergeCell ref="Y46:Y47"/>
+    <mergeCell ref="Y48:Y49"/>
+    <mergeCell ref="Y38:Y39"/>
+    <mergeCell ref="Y40:Y41"/>
+    <mergeCell ref="Z60:Z61"/>
+    <mergeCell ref="Z62:Z63"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Y14:Y15"/>
+    <mergeCell ref="Y26:Y27"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="Y30:Y31"/>
+    <mergeCell ref="Y32:Y33"/>
+    <mergeCell ref="Y34:Y35"/>
+    <mergeCell ref="Y36:Y37"/>
+    <mergeCell ref="Y12:Y13"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="Y18:Y19"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="Z14:Z15"/>
+    <mergeCell ref="Z26:Z27"/>
+    <mergeCell ref="Z28:Z29"/>
+    <mergeCell ref="Z30:Z31"/>
+    <mergeCell ref="Z32:Z33"/>
+    <mergeCell ref="Z34:Z35"/>
+    <mergeCell ref="Z36:Z37"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="Z18:Z19"/>
+    <mergeCell ref="Z50:Z51"/>
+    <mergeCell ref="Z52:Z53"/>
+    <mergeCell ref="Z54:Z55"/>
+    <mergeCell ref="Z56:Z57"/>
+    <mergeCell ref="Z58:Z59"/>
+    <mergeCell ref="Z42:Z43"/>
+    <mergeCell ref="Z44:Z45"/>
+    <mergeCell ref="Z46:Z47"/>
+    <mergeCell ref="Z48:Z49"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="W12:W13"/>
+    <mergeCell ref="X12:X13"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="X16:X17"/>
+    <mergeCell ref="W18:W19"/>
+    <mergeCell ref="X18:X19"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="C16:C35"/>
+    <mergeCell ref="C36:C41"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="W20:W21"/>
+    <mergeCell ref="X20:X21"/>
+    <mergeCell ref="Y20:Y21"/>
+    <mergeCell ref="Z20:Z21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="Y22:Y23"/>
+    <mergeCell ref="Z22:Z23"/>
+    <mergeCell ref="Z38:Z39"/>
+    <mergeCell ref="Z40:Z41"/>
+    <mergeCell ref="X40:X41"/>
+    <mergeCell ref="W26:W27"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="Y24:Y25"/>
+    <mergeCell ref="X60:X61"/>
+    <mergeCell ref="X62:X63"/>
+    <mergeCell ref="X50:X51"/>
+    <mergeCell ref="X52:X53"/>
+    <mergeCell ref="X54:X55"/>
+    <mergeCell ref="X56:X57"/>
+    <mergeCell ref="X58:X59"/>
+    <mergeCell ref="Y60:Y61"/>
+    <mergeCell ref="Y62:Y63"/>
+    <mergeCell ref="Y50:Y51"/>
+    <mergeCell ref="Y52:Y53"/>
+    <mergeCell ref="Y54:Y55"/>
+    <mergeCell ref="Y56:Y57"/>
+    <mergeCell ref="Y58:Y59"/>
+    <mergeCell ref="Y42:Y43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>